<commit_message>
deposits happen while age strictly less than retirement age
</commit_message>
<xml_diff>
--- a/doc/testCases.xlsx
+++ b/doc/testCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus Enrique\repos\final-project-retirement-planner\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89845032-1A7D-4BAB-87CD-494AF8169F62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C06BB1-8272-4E09-97DA-ED129C8B13EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{AFEE7A28-A0EB-4DDF-92DA-2882173264C8}"/>
+    <workbookView xWindow="22335" yWindow="0" windowWidth="16065" windowHeight="15600" xr2:uid="{AFEE7A28-A0EB-4DDF-92DA-2882173264C8}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase 1" sheetId="1" r:id="rId1"/>
@@ -128,11 +128,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -450,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBD3B8D-B490-4E50-B529-2AF514893D3A}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -568,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="D13:D44" si="1">IF(A13&lt;=$B$4,$B$8,-$B$9)</f>
+        <f>IF(A13&lt;$B$4,$B$8,-$B$9)</f>
         <v>10000</v>
       </c>
     </row>
@@ -586,7 +588,7 @@
         <v>194.17475728155341</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D14:D77" si="1">IF(A14&lt;$B$4,$B$8,-$B$9)</f>
         <v>10000</v>
       </c>
     </row>
@@ -1109,7 +1111,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>-25000</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1119,11 +1121,11 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" si="3"/>
-        <v>419806.09282522125</v>
+        <v>384806.09282522125</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" si="0"/>
-        <v>8151.5746179654616</v>
+        <v>7471.9629674800253</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" si="1"/>
@@ -1137,14 +1139,14 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" si="3"/>
-        <v>402957.66744318668</v>
+        <v>367278.05579270126</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" ref="C45:C76" si="4">B45*$B$7</f>
-        <v>7824.4207270521692</v>
+        <v>7131.6127338388596</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" ref="D45:D76" si="5">IF(A45&lt;=$B$4,$B$8,-$B$9)</f>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1155,14 +1157,14 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" si="3"/>
-        <v>385782.08817023883</v>
+        <v>349409.6685265401</v>
       </c>
       <c r="C46" s="1">
         <f t="shared" si="4"/>
-        <v>7490.9143334026967</v>
+        <v>6784.6537577968957</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1173,14 +1175,14 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" si="3"/>
-        <v>368273.00250364153</v>
+        <v>331194.32228433702</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" si="4"/>
-        <v>7150.9320874493505</v>
+        <v>6430.9577142589715</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1191,14 +1193,14 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" si="3"/>
-        <v>350423.93459109089</v>
+        <v>312625.279998596</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" si="4"/>
-        <v>6804.3482444872025</v>
+        <v>6070.3937863805058</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1209,14 +1211,14 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" si="3"/>
-        <v>332228.28283557808</v>
+        <v>293695.67378497653</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" si="4"/>
-        <v>6451.0346181665655</v>
+        <v>5702.8286171840109</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1227,14 +1229,14 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" si="3"/>
-        <v>313679.31745374465</v>
+        <v>274398.50240216055</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" si="4"/>
-        <v>6090.8605330824212</v>
+        <v>5328.1262602361276</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1245,14 +1247,14 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" si="3"/>
-        <v>294770.1779868271</v>
+        <v>254726.62866239669</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" si="4"/>
-        <v>5723.6927764432448</v>
+        <v>4946.1481293669267</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1263,32 +1265,32 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" si="3"/>
-        <v>275493.87076327036</v>
+        <v>234672.77679176361</v>
       </c>
       <c r="C52" s="1">
         <f t="shared" si="4"/>
-        <v>5349.3955488013671</v>
+        <v>4556.752947412886</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="2">
+      <c r="A53" s="4">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B53" s="3">
-        <f t="shared" si="3"/>
-        <v>255843.2663120717</v>
-      </c>
-      <c r="C53" s="3">
-        <f t="shared" si="4"/>
-        <v>4967.8304138266358</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="5"/>
+      <c r="B53" s="5">
+        <f t="shared" si="3"/>
+        <v>214229.52973917651</v>
+      </c>
+      <c r="C53" s="5">
+        <f t="shared" si="4"/>
+        <v>4159.796693964593</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1299,14 +1301,14 @@
       </c>
       <c r="B54" s="1">
         <f t="shared" si="3"/>
-        <v>235811.09672589833</v>
+        <v>193389.3264331411</v>
       </c>
       <c r="C54" s="1">
         <f t="shared" si="4"/>
-        <v>4578.8562471048226</v>
+        <v>3755.1325520998275</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1317,14 +1319,14 @@
       </c>
       <c r="B55" s="1">
         <f t="shared" si="3"/>
-        <v>215389.95297300315</v>
+        <v>172144.45898524093</v>
       </c>
       <c r="C55" s="1">
         <f t="shared" si="4"/>
-        <v>4182.3291839418089</v>
+        <v>3342.6108540823484</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1335,14 +1337,14 @@
       </c>
       <c r="B56" s="1">
         <f t="shared" si="3"/>
-        <v>194572.28215694497</v>
+        <v>150487.06983932329</v>
       </c>
       <c r="C56" s="1">
         <f t="shared" si="4"/>
-        <v>3778.1025661542717</v>
+        <v>2922.0790260062777</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1353,14 +1355,14 @@
       </c>
       <c r="B57" s="1">
         <f t="shared" si="3"/>
-        <v>173350.38472309924</v>
+        <v>128409.14886532957</v>
       </c>
       <c r="C57" s="1">
         <f t="shared" si="4"/>
-        <v>3366.02688782717</v>
+        <v>2493.3815313656228</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1371,14 +1373,14 @@
       </c>
       <c r="B58" s="1">
         <f t="shared" si="3"/>
-        <v>151716.41161092641</v>
+        <v>105902.53039669519</v>
       </c>
       <c r="C58" s="1">
         <f t="shared" si="4"/>
-        <v>2945.9497400179889</v>
+        <v>2056.3598135280622</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1389,14 +1391,14 @@
       </c>
       <c r="B59" s="1">
         <f t="shared" si="3"/>
-        <v>129662.36135094441</v>
+        <v>82958.890210223253</v>
       </c>
       <c r="C59" s="1">
         <f t="shared" si="4"/>
-        <v>2517.7157543872704</v>
+        <v>1610.8522370917137</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1407,14 +1409,14 @@
       </c>
       <c r="B60" s="1">
         <f t="shared" si="3"/>
-        <v>107180.07710533167</v>
+        <v>59569.742447314973</v>
       </c>
       <c r="C60" s="1">
         <f t="shared" si="4"/>
-        <v>2081.1665457345957</v>
+        <v>1156.6940281032034</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1425,32 +1427,32 @@
       </c>
       <c r="B61" s="1">
         <f t="shared" si="3"/>
-        <v>84261.243651066266</v>
+        <v>35726.436475418173</v>
       </c>
       <c r="C61" s="1">
         <f t="shared" si="4"/>
-        <v>1636.1406534187627</v>
+        <v>693.71721311491604</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62">
+      <c r="A62" s="2">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="B62" s="1">
-        <f t="shared" si="3"/>
-        <v>60897.384304485022</v>
-      </c>
-      <c r="C62" s="1">
-        <f t="shared" si="4"/>
-        <v>1182.4734816404859</v>
-      </c>
-      <c r="D62" s="1">
-        <f t="shared" si="5"/>
+      <c r="B62" s="3">
+        <f t="shared" si="3"/>
+        <v>11420.153688533086</v>
+      </c>
+      <c r="C62" s="3">
+        <f t="shared" si="4"/>
+        <v>221.75055705889488</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1461,14 +1463,14 @@
       </c>
       <c r="B63" s="1">
         <f t="shared" si="3"/>
-        <v>37079.857786125511</v>
+        <v>-13358.095754408019</v>
       </c>
       <c r="C63" s="1">
         <f t="shared" si="4"/>
-        <v>719.99723856554397</v>
+        <v>-259.38050008559264</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1479,14 +1481,14 @@
       </c>
       <c r="B64" s="3">
         <f t="shared" si="3"/>
-        <v>12799.855024691053</v>
+        <v>-38617.476254493609</v>
       </c>
       <c r="C64" s="3">
         <f t="shared" si="4"/>
-        <v>248.5408742658457</v>
-      </c>
-      <c r="D64" s="3">
-        <f t="shared" si="5"/>
+        <v>-749.85390785424488</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1497,14 +1499,14 @@
       </c>
       <c r="B65" s="1">
         <f t="shared" si="3"/>
-        <v>-11951.604101043102</v>
+        <v>-64367.330162347855</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" si="4"/>
-        <v>-232.06998254452628</v>
+        <v>-1249.8510711135507</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1515,14 +1517,14 @@
       </c>
       <c r="B66" s="1">
         <f t="shared" si="3"/>
-        <v>-37183.674083587626</v>
+        <v>-90617.181233461408</v>
       </c>
       <c r="C66" s="1">
         <f t="shared" si="4"/>
-        <v>-722.01308900170159</v>
+        <v>-1759.5569171545906</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1533,14 +1535,14 @@
       </c>
       <c r="B67" s="1">
         <f t="shared" si="3"/>
-        <v>-62905.687172589329</v>
+        <v>-117376.738150616</v>
       </c>
       <c r="C67" s="1">
         <f t="shared" si="4"/>
-        <v>-1221.4696538366861</v>
+        <v>-2279.1599640896311</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1551,14 +1553,14 @@
       </c>
       <c r="B68" s="1">
         <f t="shared" si="3"/>
-        <v>-89127.156826426013</v>
+        <v>-144655.89811470563</v>
       </c>
       <c r="C68" s="1">
         <f t="shared" si="4"/>
-        <v>-1730.6244043966217</v>
+        <v>-2808.8523905768088</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1569,14 +1571,14 @@
       </c>
       <c r="B69" s="1">
         <f t="shared" si="3"/>
-        <v>-115857.78123082264</v>
+        <v>-172464.75050528243</v>
       </c>
       <c r="C69" s="1">
         <f t="shared" si="4"/>
-        <v>-2249.6656549674303</v>
+        <v>-3348.8301068986884</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1587,14 +1589,14 @@
       </c>
       <c r="B70" s="1">
         <f t="shared" si="3"/>
-        <v>-143107.44688579009</v>
+        <v>-200813.5806121811</v>
       </c>
       <c r="C70" s="1">
         <f t="shared" si="4"/>
-        <v>-2778.785376423109</v>
+        <v>-3899.2928274209926</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1605,14 +1607,14 @@
       </c>
       <c r="B71" s="1">
         <f t="shared" si="3"/>
-        <v>-170886.23226221319</v>
+        <v>-229712.87343960209</v>
       </c>
       <c r="C71" s="1">
         <f t="shared" si="4"/>
-        <v>-3318.179267227441</v>
+        <v>-4460.4441444582935</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1623,14 +1625,14 @@
       </c>
       <c r="B72" s="1">
         <f t="shared" si="3"/>
-        <v>-199204.41152944064</v>
+        <v>-259173.31758406039</v>
       </c>
       <c r="C72" s="1">
         <f t="shared" si="4"/>
-        <v>-3868.0468258143815</v>
+        <v>-5032.4916035739889</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1641,14 +1643,14 @@
       </c>
       <c r="B73" s="1">
         <f t="shared" si="3"/>
-        <v>-228072.45835525502</v>
+        <v>-289205.80918763438</v>
       </c>
       <c r="C73" s="1">
         <f t="shared" si="4"/>
-        <v>-4428.5914243738844</v>
+        <v>-5615.6467803424157</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1659,14 +1661,14 @@
       </c>
       <c r="B74" s="1">
         <f t="shared" si="3"/>
-        <v>-257501.0497796289</v>
+        <v>-319821.45596797677</v>
       </c>
       <c r="C74" s="1">
         <f t="shared" si="4"/>
-        <v>-5000.0203840704644</v>
+        <v>-6210.1253586014909</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1677,14 +1679,14 @@
       </c>
       <c r="B75" s="1">
         <f t="shared" si="3"/>
-        <v>-287501.07016369939</v>
+        <v>-351031.58132657828</v>
       </c>
       <c r="C75" s="1">
         <f t="shared" si="4"/>
-        <v>-5582.5450517223189</v>
+        <v>-6816.1472102248217</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1695,14 +1697,14 @@
       </c>
       <c r="B76" s="1">
         <f t="shared" si="3"/>
-        <v>-318083.61521542171</v>
+        <v>-382847.7285368031</v>
       </c>
       <c r="C76" s="1">
         <f t="shared" si="4"/>
-        <v>-6176.3808779693545</v>
+        <v>-7433.9364764427792</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1713,14 +1715,14 @@
       </c>
       <c r="B77" s="1">
         <f t="shared" si="3"/>
-        <v>-349259.99609339109</v>
+        <v>-415281.66501324589</v>
       </c>
       <c r="C77" s="1">
-        <f t="shared" ref="C77" si="6">B77*$B$7</f>
-        <v>-6781.7474969590512</v>
+        <f t="shared" ref="C77" si="5">B77*$B$7</f>
+        <v>-8063.7216507426392</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" ref="D77:D88" si="7">IF(A77&lt;=$B$4,$B$8,-$B$9)</f>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -1731,29 +1733,29 @@
       </c>
       <c r="B78" s="1">
         <f t="shared" si="3"/>
-        <v>-381041.74359035015</v>
+        <v>-448345.38666398852</v>
       </c>
       <c r="C78" s="1">
-        <f t="shared" ref="C78:C88" si="8">B78*$B$7</f>
-        <v>-7398.8688075796153</v>
+        <f t="shared" ref="C78:C88" si="6">B78*$B$7</f>
+        <v>-8705.7356633784184</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="D78:D88" si="7">IF(A78&lt;$B$4,$B$8,-$B$9)</f>
         <v>-25000</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
-        <f t="shared" ref="A79:A88" si="9">A78+1</f>
+        <f t="shared" ref="A79:A88" si="8">A78+1</f>
         <v>96</v>
       </c>
       <c r="B79" s="1">
         <f t="shared" si="3"/>
-        <v>-413440.61239792977</v>
+        <v>-482051.12232736696</v>
       </c>
       <c r="C79" s="1">
-        <f t="shared" si="8"/>
-        <v>-8027.9730562704817</v>
+        <f t="shared" si="6"/>
+        <v>-9360.2159675216899</v>
       </c>
       <c r="D79" s="1">
         <f t="shared" si="7"/>
@@ -1762,16 +1764,16 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>97</v>
       </c>
       <c r="B80" s="1">
-        <f t="shared" ref="B80:B88" si="10">B79+C79+D79</f>
-        <v>-446468.58545420028</v>
+        <f t="shared" ref="B80:B88" si="9">B79+C79+D79</f>
+        <v>-516411.33829488867</v>
       </c>
       <c r="C80" s="1">
-        <f t="shared" si="8"/>
-        <v>-8669.2929214407832</v>
+        <f t="shared" si="6"/>
+        <v>-10027.404627085218</v>
       </c>
       <c r="D80" s="1">
         <f t="shared" si="7"/>
@@ -1780,16 +1782,16 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="B81" s="1">
         <f t="shared" si="9"/>
-        <v>98</v>
-      </c>
-      <c r="B81" s="1">
-        <f t="shared" si="10"/>
-        <v>-480137.87837564107</v>
+        <v>-551438.74292197393</v>
       </c>
       <c r="C81" s="1">
-        <f t="shared" si="8"/>
-        <v>-9323.0655995270117</v>
+        <f t="shared" si="6"/>
+        <v>-10707.548406251923</v>
       </c>
       <c r="D81" s="1">
         <f t="shared" si="7"/>
@@ -1798,16 +1800,16 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
+        <f t="shared" si="8"/>
+        <v>99</v>
+      </c>
+      <c r="B82" s="1">
         <f t="shared" si="9"/>
-        <v>99</v>
-      </c>
-      <c r="B82" s="1">
-        <f t="shared" si="10"/>
-        <v>-514460.94397516811</v>
+        <v>-587146.29132822587</v>
       </c>
       <c r="C82" s="1">
-        <f t="shared" si="8"/>
-        <v>-9989.5328927217124</v>
+        <f t="shared" si="6"/>
+        <v>-11400.898860742251</v>
       </c>
       <c r="D82" s="1">
         <f t="shared" si="7"/>
@@ -1816,16 +1818,16 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="B83" s="1">
         <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-      <c r="B83" s="1">
-        <f t="shared" si="10"/>
-        <v>-549450.47686788987</v>
+        <v>-623547.19018896809</v>
       </c>
       <c r="C83" s="1">
-        <f t="shared" si="8"/>
-        <v>-10668.941298405629</v>
+        <f t="shared" si="6"/>
+        <v>-12107.71243085375</v>
       </c>
       <c r="D83" s="1">
         <f t="shared" si="7"/>
@@ -1834,16 +1836,16 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
+        <f t="shared" si="8"/>
+        <v>101</v>
+      </c>
+      <c r="B84" s="1">
         <f t="shared" si="9"/>
-        <v>101</v>
-      </c>
-      <c r="B84" s="1">
-        <f t="shared" si="10"/>
-        <v>-585119.41816629551</v>
+        <v>-660654.90261982183</v>
       </c>
       <c r="C84" s="1">
-        <f t="shared" si="8"/>
-        <v>-11361.542100316419</v>
+        <f t="shared" si="6"/>
+        <v>-12828.250536307221</v>
       </c>
       <c r="D84" s="1">
         <f t="shared" si="7"/>
@@ -1852,16 +1854,16 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
+        <f t="shared" si="8"/>
+        <v>102</v>
+      </c>
+      <c r="B85" s="1">
         <f t="shared" si="9"/>
-        <v>102</v>
-      </c>
-      <c r="B85" s="1">
-        <f t="shared" si="10"/>
-        <v>-621480.96026661189</v>
+        <v>-698483.15315612906</v>
       </c>
       <c r="C85" s="1">
-        <f t="shared" si="8"/>
-        <v>-12067.591461487611</v>
+        <f t="shared" si="6"/>
+        <v>-13562.779672934546</v>
       </c>
       <c r="D85" s="1">
         <f t="shared" si="7"/>
@@ -1870,16 +1872,16 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
+        <f t="shared" si="8"/>
+        <v>103</v>
+      </c>
+      <c r="B86" s="1">
         <f t="shared" si="9"/>
-        <v>103</v>
-      </c>
-      <c r="B86" s="1">
-        <f t="shared" si="10"/>
-        <v>-658548.55172809947</v>
+        <v>-737045.93282906362</v>
       </c>
       <c r="C86" s="1">
-        <f t="shared" si="8"/>
-        <v>-12787.350518992223</v>
+        <f t="shared" si="6"/>
+        <v>-14311.571511243956</v>
       </c>
       <c r="D86" s="1">
         <f t="shared" si="7"/>
@@ -1888,16 +1890,16 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
+        <f t="shared" si="8"/>
+        <v>104</v>
+      </c>
+      <c r="B87" s="1">
         <f t="shared" si="9"/>
-        <v>104</v>
-      </c>
-      <c r="B87" s="1">
-        <f t="shared" si="10"/>
-        <v>-696335.90224709164</v>
+        <v>-776357.50434030755</v>
       </c>
       <c r="C87" s="1">
-        <f t="shared" si="8"/>
-        <v>-13521.085480526053</v>
+        <f t="shared" si="6"/>
+        <v>-15074.902996899178</v>
       </c>
       <c r="D87" s="1">
         <f t="shared" si="7"/>
@@ -1906,16 +1908,16 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
+        <f t="shared" si="8"/>
+        <v>105</v>
+      </c>
+      <c r="B88" s="1">
         <f t="shared" si="9"/>
-        <v>105</v>
-      </c>
-      <c r="B88" s="1">
-        <f t="shared" si="10"/>
-        <v>-734856.98772761773</v>
+        <v>-816432.40733720677</v>
       </c>
       <c r="C88" s="1">
-        <f t="shared" si="8"/>
-        <v>-14269.067722866364</v>
+        <f t="shared" si="6"/>
+        <v>-15853.056453149647</v>
       </c>
       <c r="D88" s="1">
         <f t="shared" si="7"/>
@@ -1931,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC81894-8DD9-4214-A8DC-DC245F1F12DD}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -2049,7 +2051,7 @@
         <v>-1941.7475728155334</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="D13:D44" si="1">IF(A13&lt;=$B$4,$B$8,-$B$9)</f>
+        <f>IF(A13&lt;$B$4,$B$8,-$B$9)</f>
         <v>0</v>
       </c>
     </row>
@@ -2067,7 +2069,7 @@
         <v>-1922.8956546328584</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D14:D77" si="1">IF(A14&lt;$B$4,$B$8,-$B$9)</f>
         <v>0</v>
       </c>
     </row>
@@ -2590,7 +2592,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-25000</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -2600,11 +2602,11 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" si="3"/>
-        <v>147802.35517150821</v>
+        <v>122802.35517150821</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" si="0"/>
-        <v>-1434.9743220534774</v>
+        <v>-1192.2558754515358</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" si="1"/>
@@ -2618,14 +2620,14 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" si="3"/>
-        <v>121367.38084945473</v>
+        <v>96610.09929605668</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" ref="C45:C76" si="4">B45*$B$7</f>
-        <v>-1178.324085917036</v>
+        <v>-937.9621290879287</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" ref="D45:D76" si="5">IF(A45&lt;=$B$4,$B$8,-$B$9)</f>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2636,14 +2638,14 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" si="3"/>
-        <v>95189.056763537694</v>
+        <v>70672.137166968751</v>
       </c>
       <c r="C46" s="1">
         <f t="shared" si="4"/>
-        <v>-924.16559964599674</v>
+        <v>-686.13725404824015</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2654,14 +2656,14 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" si="3"/>
-        <v>69264.891163891691</v>
+        <v>44985.99991292051</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" si="4"/>
-        <v>-672.47467149409385</v>
+        <v>-436.757280707966</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2672,14 +2674,14 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" si="3"/>
-        <v>43592.416492397591</v>
+        <v>19549.242632212547</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" si="4"/>
-        <v>-423.22734458638428</v>
+        <v>-189.79847215740332</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2690,14 +2692,14 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" si="3"/>
-        <v>18169.189147811208</v>
+        <v>-5640.5558399448564</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" si="4"/>
-        <v>-176.39989463894372</v>
+        <v>54.762678057717039</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2708,14 +2710,14 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" si="3"/>
-        <v>-7007.2107468277354</v>
+        <v>-30585.793161887137</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" si="4"/>
-        <v>68.03117229929839</v>
+        <v>296.94944817366144</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2726,14 +2728,14 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" si="3"/>
-        <v>-31939.179574528436</v>
+        <v>-55288.843713713475</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" si="4"/>
-        <v>310.08912208280026</v>
+        <v>536.78489042440253</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2744,14 +2746,14 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" si="3"/>
-        <v>-56629.090452445635</v>
+        <v>-79752.058823289073</v>
       </c>
       <c r="C52" s="1">
         <f t="shared" si="4"/>
-        <v>549.79699468393801</v>
+        <v>774.29183323581606</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2762,14 +2764,14 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" si="3"/>
-        <v>-81079.293457761698</v>
+        <v>-103977.76699005326</v>
       </c>
       <c r="C53" s="1">
         <f t="shared" si="4"/>
-        <v>787.17760638603568</v>
+        <v>1009.4928833985751</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2780,14 +2782,14 @@
       </c>
       <c r="B54" s="1">
         <f t="shared" si="3"/>
-        <v>-105292.11585137567</v>
+        <v>-127968.27410665469</v>
       </c>
       <c r="C54" s="1">
         <f t="shared" si="4"/>
-        <v>1022.2535519551033</v>
+        <v>1242.410428219948</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2798,14 +2800,14 @@
       </c>
       <c r="B55" s="1">
         <f t="shared" si="3"/>
-        <v>-129269.86229942057</v>
+        <v>-151725.86367843475</v>
       </c>
       <c r="C55" s="1">
         <f t="shared" si="4"/>
-        <v>1255.0472067904907</v>
+        <v>1473.0666376547058</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2816,14 +2818,14 @@
       </c>
       <c r="B56" s="1">
         <f t="shared" si="3"/>
-        <v>-153014.81509263007</v>
+        <v>-175252.79704078005</v>
       </c>
       <c r="C56" s="1">
         <f t="shared" si="4"/>
-        <v>1485.5807290546604</v>
+        <v>1701.4834664153398</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2834,14 +2836,14 @@
       </c>
       <c r="B57" s="1">
         <f t="shared" si="3"/>
-        <v>-176529.23436357541</v>
+        <v>-198551.3135743647</v>
       </c>
       <c r="C57" s="1">
         <f t="shared" si="4"/>
-        <v>1713.876061782285</v>
+        <v>1927.6826560617926</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2852,14 +2854,14 @@
       </c>
       <c r="B58" s="1">
         <f t="shared" si="3"/>
-        <v>-199815.35830179311</v>
+        <v>-221623.63091830289</v>
       </c>
       <c r="C58" s="1">
         <f t="shared" si="4"/>
-        <v>1939.9549349688646</v>
+        <v>2151.6857370709013</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2870,14 +2872,14 @@
       </c>
       <c r="B59" s="1">
         <f t="shared" si="3"/>
-        <v>-222875.40336682423</v>
+        <v>-244471.945181232</v>
       </c>
       <c r="C59" s="1">
         <f t="shared" si="4"/>
-        <v>2163.8388676390696</v>
+        <v>2373.5140308857472</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2888,14 +2890,14 @@
       </c>
       <c r="B60" s="1">
         <f t="shared" si="3"/>
-        <v>-245711.56449918516</v>
+        <v>-267098.4311503463</v>
       </c>
       <c r="C60" s="1">
         <f t="shared" si="4"/>
-        <v>2385.5491698950009</v>
+        <v>2593.1886519451091</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2906,14 +2908,14 @@
       </c>
       <c r="B61" s="1">
         <f t="shared" si="3"/>
-        <v>-268326.01532929018</v>
+        <v>-289505.2424984012</v>
       </c>
       <c r="C61" s="1">
         <f t="shared" si="4"/>
-        <v>2605.106944944564</v>
+        <v>2810.730509693215</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2924,14 +2926,14 @@
       </c>
       <c r="B62" s="1">
         <f t="shared" si="3"/>
-        <v>-290720.90838434559</v>
+        <v>-311694.51198870799</v>
       </c>
       <c r="C62" s="1">
         <f t="shared" si="4"/>
-        <v>2822.5330911101505</v>
+        <v>3026.1603105699796</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2942,14 +2944,14 @@
       </c>
       <c r="B63" s="1">
         <f t="shared" si="3"/>
-        <v>-312898.37529323541</v>
+        <v>-333668.35167813802</v>
       </c>
       <c r="C63" s="1">
         <f t="shared" si="4"/>
-        <v>3037.8483038178188</v>
+        <v>3239.4985599819215</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2960,14 +2962,14 @@
       </c>
       <c r="B64" s="1">
         <f t="shared" si="3"/>
-        <v>-334860.52698941762</v>
+        <v>-355428.85311815608</v>
       </c>
       <c r="C64" s="1">
         <f t="shared" si="4"/>
-        <v>3251.0730775671605</v>
+        <v>3450.7655642539416</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2978,14 +2980,14 @@
       </c>
       <c r="B65" s="1">
         <f t="shared" si="3"/>
-        <v>-356609.45391185046</v>
+        <v>-376978.08755390212</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" si="4"/>
-        <v>3462.2277078820425</v>
+        <v>3659.9814325621555</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -2996,14 +2998,14 @@
       </c>
       <c r="B66" s="1">
         <f t="shared" si="3"/>
-        <v>-378147.2262039684</v>
+        <v>-398318.10612133995</v>
       </c>
       <c r="C66" s="1">
         <f t="shared" si="4"/>
-        <v>3671.3322932424107</v>
+        <v>3867.1660788479599</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3014,14 +3016,14 @@
       </c>
       <c r="B67" s="1">
         <f t="shared" si="3"/>
-        <v>-399475.89391072601</v>
+        <v>-419450.940042492</v>
       </c>
       <c r="C67" s="1">
         <f t="shared" si="4"/>
-        <v>3878.4067369973391</v>
+        <v>4072.3392237135135</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3032,14 +3034,14 @@
       </c>
       <c r="B68" s="1">
         <f t="shared" si="3"/>
-        <v>-420597.48717372864</v>
+        <v>-440378.6008187785</v>
       </c>
       <c r="C68" s="1">
         <f t="shared" si="4"/>
-        <v>4083.4707492595003</v>
+        <v>4275.5203962988189</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3050,14 +3052,14 @@
       </c>
       <c r="B69" s="1">
         <f t="shared" si="3"/>
-        <v>-441514.01642446913</v>
+        <v>-461103.08042247966</v>
       </c>
       <c r="C69" s="1">
         <f t="shared" si="4"/>
-        <v>4286.5438487812526</v>
+        <v>4476.7289361405783</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3068,14 +3070,14 @@
       </c>
       <c r="B70" s="1">
         <f t="shared" si="3"/>
-        <v>-462227.47257568786</v>
+        <v>-481626.35148633906</v>
       </c>
       <c r="C70" s="1">
         <f t="shared" si="4"/>
-        <v>4487.6453648125025</v>
+        <v>4675.983995012999</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3086,14 +3088,14 @@
       </c>
       <c r="B71" s="1">
         <f t="shared" si="3"/>
-        <v>-482739.82721087534</v>
+        <v>-501950.36749132606</v>
       </c>
       <c r="C71" s="1">
         <f t="shared" si="4"/>
-        <v>4686.7944389405357</v>
+        <v>4873.3045387507373</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3104,14 +3106,14 @@
       </c>
       <c r="B72" s="1">
         <f t="shared" si="3"/>
-        <v>-503053.03277193481</v>
+        <v>-522077.06295257533</v>
       </c>
       <c r="C72" s="1">
         <f t="shared" si="4"/>
-        <v>4884.0100269119876</v>
+        <v>5068.7093490541283</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3122,14 +3124,14 @@
       </c>
       <c r="B73" s="1">
         <f t="shared" si="3"/>
-        <v>-523169.02274502284</v>
+        <v>-542008.35360352113</v>
       </c>
       <c r="C73" s="1">
         <f t="shared" si="4"/>
-        <v>5079.3109004371136</v>
+        <v>5262.2170252769029</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3140,14 +3142,14 @@
       </c>
       <c r="B74" s="1">
         <f t="shared" si="3"/>
-        <v>-543089.71184458572</v>
+        <v>-561746.13657824427</v>
       </c>
       <c r="C74" s="1">
         <f t="shared" si="4"/>
-        <v>5272.7156489765594</v>
+        <v>5453.8459861965448</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3158,14 +3160,14 @@
       </c>
       <c r="B75" s="1">
         <f t="shared" si="3"/>
-        <v>-562816.99619560922</v>
+        <v>-581292.29059204774</v>
       </c>
       <c r="C75" s="1">
         <f t="shared" si="4"/>
-        <v>5464.2426815107674</v>
+        <v>5643.6144717674524</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3176,14 +3178,14 @@
       </c>
       <c r="B76" s="1">
         <f t="shared" si="3"/>
-        <v>-582352.75351409847</v>
+        <v>-600648.67612028029</v>
       </c>
       <c r="C76" s="1">
         <f t="shared" si="4"/>
-        <v>5653.9102282922167</v>
+        <v>5831.5405448570882</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3194,14 +3196,14 @@
       </c>
       <c r="B77" s="1">
         <f t="shared" si="3"/>
-        <v>-601698.84328580624</v>
+        <v>-619817.13557542325</v>
       </c>
       <c r="C77" s="1">
-        <f t="shared" ref="C77" si="6">B77*$B$7</f>
-        <v>5841.7363425806416</v>
+        <f t="shared" ref="C77" si="5">B77*$B$7</f>
+        <v>6017.6420929652722</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" ref="D77:D88" si="7">IF(A77&lt;=$B$4,$B$8,-$B$9)</f>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -3212,29 +3214,29 @@
       </c>
       <c r="B78" s="1">
         <f t="shared" si="3"/>
-        <v>-620857.1069432256</v>
+        <v>-638799.49348245794</v>
       </c>
       <c r="C78" s="1">
-        <f t="shared" ref="C78:C88" si="8">B78*$B$7</f>
-        <v>6027.7389023614123</v>
+        <f t="shared" ref="C78:C88" si="6">B78*$B$7</f>
+        <v>6201.9368299267744</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="D78:D88" si="7">IF(A78&lt;$B$4,$B$8,-$B$9)</f>
         <v>-25000</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
-        <f t="shared" ref="A79:A88" si="9">A78+1</f>
+        <f t="shared" ref="A79:A88" si="8">A78+1</f>
         <v>96</v>
       </c>
       <c r="B79" s="1">
         <f t="shared" si="3"/>
-        <v>-639829.36804086424</v>
+        <v>-657597.55665253114</v>
       </c>
       <c r="C79" s="1">
-        <f t="shared" si="8"/>
-        <v>6211.9356120472239</v>
+        <f t="shared" si="6"/>
+        <v>6384.4422975973885</v>
       </c>
       <c r="D79" s="1">
         <f t="shared" si="7"/>
@@ -3243,16 +3245,16 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>97</v>
       </c>
       <c r="B80" s="1">
-        <f t="shared" ref="B80:B88" si="10">B79+C79+D79</f>
-        <v>-658617.43242881703</v>
+        <f t="shared" ref="B80:B88" si="9">B79+C79+D79</f>
+        <v>-676213.11435493373</v>
       </c>
       <c r="C80" s="1">
-        <f t="shared" si="8"/>
-        <v>6394.3440041632703</v>
+        <f t="shared" si="6"/>
+        <v>6565.1758675236269</v>
       </c>
       <c r="D80" s="1">
         <f t="shared" si="7"/>
@@ -3261,16 +3263,16 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="B81" s="1">
         <f t="shared" si="9"/>
-        <v>98</v>
-      </c>
-      <c r="B81" s="1">
-        <f t="shared" si="10"/>
-        <v>-677223.08842465375</v>
+        <v>-694647.93848741008</v>
       </c>
       <c r="C81" s="1">
-        <f t="shared" si="8"/>
-        <v>6574.9814410160543</v>
+        <f t="shared" si="6"/>
+        <v>6744.1547425962126</v>
       </c>
       <c r="D81" s="1">
         <f t="shared" si="7"/>
@@ -3279,16 +3281,16 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
+        <f t="shared" si="8"/>
+        <v>99</v>
+      </c>
+      <c r="B82" s="1">
         <f t="shared" si="9"/>
-        <v>99</v>
-      </c>
-      <c r="B82" s="1">
-        <f t="shared" si="10"/>
-        <v>-695648.10698363767</v>
+        <v>-712903.78374481387</v>
       </c>
       <c r="C82" s="1">
-        <f t="shared" si="8"/>
-        <v>6753.8651163459954</v>
+        <f t="shared" si="6"/>
+        <v>6921.3959586875117</v>
       </c>
       <c r="D82" s="1">
         <f t="shared" si="7"/>
@@ -3297,16 +3299,16 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="B83" s="1">
         <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-      <c r="B83" s="1">
-        <f t="shared" si="10"/>
-        <v>-713894.24186729162</v>
+        <v>-730982.38778612635</v>
       </c>
       <c r="C83" s="1">
-        <f t="shared" si="8"/>
-        <v>6931.0120569639948</v>
+        <f t="shared" si="6"/>
+        <v>7096.9163862730693</v>
       </c>
       <c r="D83" s="1">
         <f t="shared" si="7"/>
@@ -3315,16 +3317,16 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
+        <f t="shared" si="8"/>
+        <v>101</v>
+      </c>
+      <c r="B84" s="1">
         <f t="shared" si="9"/>
-        <v>101</v>
-      </c>
-      <c r="B84" s="1">
-        <f t="shared" si="10"/>
-        <v>-731963.22981032764</v>
+        <v>-748885.47139985324</v>
       </c>
       <c r="C84" s="1">
-        <f t="shared" si="8"/>
-        <v>7106.4391243721111</v>
+        <f t="shared" si="6"/>
+        <v>7270.7327320374079</v>
       </c>
       <c r="D84" s="1">
         <f t="shared" si="7"/>
@@ -3333,16 +3335,16 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
+        <f t="shared" si="8"/>
+        <v>102</v>
+      </c>
+      <c r="B85" s="1">
         <f t="shared" si="9"/>
-        <v>102</v>
-      </c>
-      <c r="B85" s="1">
-        <f t="shared" si="10"/>
-        <v>-749856.79068595555</v>
+        <v>-766614.73866781581</v>
       </c>
       <c r="C85" s="1">
-        <f t="shared" si="8"/>
-        <v>7280.1630163684986</v>
+        <f t="shared" si="6"/>
+        <v>7442.8615404642287</v>
       </c>
       <c r="D85" s="1">
         <f t="shared" si="7"/>
@@ -3351,16 +3353,16 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
+        <f t="shared" si="8"/>
+        <v>103</v>
+      </c>
+      <c r="B86" s="1">
         <f t="shared" si="9"/>
-        <v>103</v>
-      </c>
-      <c r="B86" s="1">
-        <f t="shared" si="10"/>
-        <v>-767576.62766958703</v>
+        <v>-784171.87712735159</v>
       </c>
       <c r="C86" s="1">
-        <f t="shared" si="8"/>
-        <v>7452.200268636765</v>
+        <f t="shared" si="6"/>
+        <v>7613.319195411178</v>
       </c>
       <c r="D86" s="1">
         <f t="shared" si="7"/>
@@ -3369,16 +3371,16 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
+        <f t="shared" si="8"/>
+        <v>104</v>
+      </c>
+      <c r="B87" s="1">
         <f t="shared" si="9"/>
-        <v>104</v>
-      </c>
-      <c r="B87" s="1">
-        <f t="shared" si="10"/>
-        <v>-785124.42740095023</v>
+        <v>-801558.55793194042</v>
       </c>
       <c r="C87" s="1">
-        <f t="shared" si="8"/>
-        <v>7622.5672563199032</v>
+        <f t="shared" si="6"/>
+        <v>7782.1219216693225</v>
       </c>
       <c r="D87" s="1">
         <f t="shared" si="7"/>
@@ -3387,16 +3389,16 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
+        <f t="shared" si="8"/>
+        <v>105</v>
+      </c>
+      <c r="B88" s="1">
         <f t="shared" si="9"/>
-        <v>105</v>
-      </c>
-      <c r="B88" s="1">
-        <f t="shared" si="10"/>
-        <v>-802501.86014463031</v>
+        <v>-818776.43601027108</v>
       </c>
       <c r="C88" s="1">
-        <f t="shared" si="8"/>
-        <v>7791.2801955789328</v>
+        <f t="shared" si="6"/>
+        <v>7949.2857865074839</v>
       </c>
       <c r="D88" s="1">
         <f t="shared" si="7"/>
@@ -3412,8 +3414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB242607-55C7-46BE-BAC1-D002E451541C}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -3530,7 +3532,7 @@
         <v>3000</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="D13:D76" si="1">IF(A13&lt;=$B$4,$B$8,-$B$9)</f>
+        <f>IF(A13&lt;$B$4,$B$8,-$B$9)</f>
         <v>10000</v>
       </c>
     </row>
@@ -3548,7 +3550,7 @@
         <v>3390</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D14:D77" si="1">IF(A14&lt;$B$4,$B$8,-$B$9)</f>
         <v>10000</v>
       </c>
     </row>
@@ -4071,7 +4073,7 @@
       </c>
       <c r="D43" s="1">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>-25000</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -4081,11 +4083,11 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" si="3"/>
-        <v>750034.81630765169</v>
+        <v>715034.81630765169</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" si="0"/>
-        <v>22501.044489229549</v>
+        <v>21451.044489229549</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" si="1"/>
@@ -4099,11 +4101,11 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" si="3"/>
-        <v>747535.86079688126</v>
+        <v>711485.86079688126</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" si="0"/>
-        <v>22426.075823906438</v>
+        <v>21344.575823906438</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" si="1"/>
@@ -4117,11 +4119,11 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" si="3"/>
-        <v>744961.93662078772</v>
+        <v>707830.43662078772</v>
       </c>
       <c r="C46" s="1">
         <f t="shared" si="0"/>
-        <v>22348.85809862363</v>
+        <v>21234.913098623631</v>
       </c>
       <c r="D46" s="1">
         <f t="shared" si="1"/>
@@ -4135,11 +4137,11 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" si="3"/>
-        <v>742310.79471941129</v>
+        <v>704065.34971941134</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" si="0"/>
-        <v>22269.323841582336</v>
+        <v>21121.96049158234</v>
       </c>
       <c r="D47" s="1">
         <f t="shared" si="1"/>
@@ -4153,11 +4155,11 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" si="3"/>
-        <v>739580.11856099358</v>
+        <v>700187.31021099363</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" si="0"/>
-        <v>22187.403556829806</v>
+        <v>21005.619306329809</v>
       </c>
       <c r="D48" s="1">
         <f t="shared" si="1"/>
@@ -4171,11 +4173,11 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" si="3"/>
-        <v>736767.52211782336</v>
+        <v>696192.92951732338</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" si="0"/>
-        <v>22103.0256635347</v>
+        <v>20885.787885519701</v>
       </c>
       <c r="D49" s="1">
         <f t="shared" si="1"/>
@@ -4189,11 +4191,11 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" si="3"/>
-        <v>733870.54778135801</v>
+        <v>692078.71740284306</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" si="0"/>
-        <v>22016.11643344074</v>
+        <v>20762.361522085292</v>
       </c>
       <c r="D50" s="1">
         <f t="shared" si="1"/>
@@ -4207,11 +4209,11 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" si="3"/>
-        <v>730886.66421479871</v>
+        <v>687841.07892492833</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" si="0"/>
-        <v>21926.59992644396</v>
+        <v>20635.232367747849</v>
       </c>
       <c r="D51" s="1">
         <f t="shared" si="1"/>
@@ -4225,11 +4227,11 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" si="3"/>
-        <v>727813.26414124272</v>
+        <v>683476.31129267614</v>
       </c>
       <c r="C52" s="1">
         <f t="shared" si="0"/>
-        <v>21834.397924237281</v>
+        <v>20504.289338780283</v>
       </c>
       <c r="D52" s="1">
         <f t="shared" si="1"/>
@@ -4243,11 +4245,11 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" si="3"/>
-        <v>724647.66206548002</v>
+        <v>678980.60063145647</v>
       </c>
       <c r="C53" s="1">
         <f t="shared" si="0"/>
-        <v>21739.4298619644</v>
+        <v>20369.418018943692</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" si="1"/>
@@ -4261,11 +4263,11 @@
       </c>
       <c r="B54" s="1">
         <f t="shared" si="3"/>
-        <v>721387.09192744445</v>
+        <v>674350.01865040022</v>
       </c>
       <c r="C54" s="1">
         <f t="shared" si="0"/>
-        <v>21641.612757823332</v>
+        <v>20230.500559512006</v>
       </c>
       <c r="D54" s="1">
         <f t="shared" si="1"/>
@@ -4279,11 +4281,11 @@
       </c>
       <c r="B55" s="1">
         <f t="shared" si="3"/>
-        <v>718028.70468526776</v>
+        <v>669580.51920991228</v>
       </c>
       <c r="C55" s="1">
         <f t="shared" si="0"/>
-        <v>21540.86114055803</v>
+        <v>20087.415576297368</v>
       </c>
       <c r="D55" s="1">
         <f t="shared" si="1"/>
@@ -4297,11 +4299,11 @@
       </c>
       <c r="B56" s="1">
         <f t="shared" si="3"/>
-        <v>714569.56582582579</v>
+        <v>664667.9347862096</v>
       </c>
       <c r="C56" s="1">
         <f t="shared" si="0"/>
-        <v>21437.086974774775</v>
+        <v>19940.038043586286</v>
       </c>
       <c r="D56" s="1">
         <f t="shared" si="1"/>
@@ -4315,11 +4317,11 @@
       </c>
       <c r="B57" s="1">
         <f t="shared" si="3"/>
-        <v>711006.65280060051</v>
+        <v>659607.97282979591</v>
       </c>
       <c r="C57" s="1">
         <f t="shared" si="0"/>
-        <v>21330.199584018013</v>
+        <v>19788.239184893875</v>
       </c>
       <c r="D57" s="1">
         <f t="shared" si="1"/>
@@ -4333,11 +4335,11 @@
       </c>
       <c r="B58" s="1">
         <f t="shared" si="3"/>
-        <v>707336.85238461848</v>
+        <v>654396.21201468981</v>
       </c>
       <c r="C58" s="1">
         <f t="shared" si="0"/>
-        <v>21220.105571538556</v>
+        <v>19631.886360440694</v>
       </c>
       <c r="D58" s="1">
         <f t="shared" si="1"/>
@@ -4351,11 +4353,11 @@
       </c>
       <c r="B59" s="1">
         <f t="shared" si="3"/>
-        <v>703556.95795615704</v>
+        <v>649028.09837513044</v>
       </c>
       <c r="C59" s="1">
         <f t="shared" si="0"/>
-        <v>21106.708738684709</v>
+        <v>19470.842951253911</v>
       </c>
       <c r="D59" s="1">
         <f t="shared" si="1"/>
@@ -4369,11 +4371,11 @@
       </c>
       <c r="B60" s="1">
         <f t="shared" si="3"/>
-        <v>699663.6666948417</v>
+        <v>643498.94132638432</v>
       </c>
       <c r="C60" s="1">
         <f t="shared" si="0"/>
-        <v>20989.910000845251</v>
+        <v>19304.968239791528</v>
       </c>
       <c r="D60" s="1">
         <f t="shared" si="1"/>
@@ -4387,11 +4389,11 @@
       </c>
       <c r="B61" s="1">
         <f t="shared" si="3"/>
-        <v>695653.5766956869</v>
+        <v>637803.90956617589</v>
       </c>
       <c r="C61" s="1">
         <f t="shared" si="0"/>
-        <v>20869.607300870608</v>
+        <v>19134.117286985274</v>
       </c>
       <c r="D61" s="1">
         <f t="shared" si="1"/>
@@ -4405,11 +4407,11 @@
       </c>
       <c r="B62" s="1">
         <f t="shared" si="3"/>
-        <v>691523.18399655749</v>
+        <v>631938.02685316117</v>
       </c>
       <c r="C62" s="1">
         <f t="shared" si="0"/>
-        <v>20745.695519896723</v>
+        <v>18958.140805594834</v>
       </c>
       <c r="D62" s="1">
         <f t="shared" si="1"/>
@@ -4423,11 +4425,11 @@
       </c>
       <c r="B63" s="1">
         <f t="shared" si="3"/>
-        <v>687268.87951645418</v>
+        <v>625896.16765875602</v>
       </c>
       <c r="C63" s="1">
         <f t="shared" si="0"/>
-        <v>20618.066385493625</v>
+        <v>18776.885029762681</v>
       </c>
       <c r="D63" s="1">
         <f t="shared" si="1"/>
@@ -4441,11 +4443,11 @@
       </c>
       <c r="B64" s="1">
         <f t="shared" si="3"/>
-        <v>682886.94590194779</v>
+        <v>619673.05268851866</v>
       </c>
       <c r="C64" s="1">
         <f t="shared" si="0"/>
-        <v>20486.608377058434</v>
+        <v>18590.191580655559</v>
       </c>
       <c r="D64" s="1">
         <f t="shared" si="1"/>
@@ -4459,11 +4461,11 @@
       </c>
       <c r="B65" s="1">
         <f t="shared" si="3"/>
-        <v>678373.5542790062</v>
+        <v>613263.24426917417</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" si="0"/>
-        <v>20351.206628370186</v>
+        <v>18397.897328075225</v>
       </c>
       <c r="D65" s="1">
         <f t="shared" si="1"/>
@@ -4477,11 +4479,11 @@
       </c>
       <c r="B66" s="1">
         <f t="shared" si="3"/>
-        <v>673724.76090737642</v>
+        <v>606661.14159724943</v>
       </c>
       <c r="C66" s="1">
         <f t="shared" si="0"/>
-        <v>20211.742827221293</v>
+        <v>18199.834247917483</v>
       </c>
       <c r="D66" s="1">
         <f t="shared" si="1"/>
@@ -4495,11 +4497,11 @@
       </c>
       <c r="B67" s="1">
         <f t="shared" si="3"/>
-        <v>668936.5037345977</v>
+        <v>599860.97584516695</v>
       </c>
       <c r="C67" s="1">
         <f t="shared" si="0"/>
-        <v>20068.095112037929</v>
+        <v>17995.829275355009</v>
       </c>
       <c r="D67" s="1">
         <f t="shared" si="1"/>
@@ -4513,11 +4515,11 @@
       </c>
       <c r="B68" s="1">
         <f t="shared" si="3"/>
-        <v>664004.59884663566</v>
+        <v>592856.80512052192</v>
       </c>
       <c r="C68" s="1">
         <f t="shared" si="0"/>
-        <v>19920.13796539907</v>
+        <v>17785.704153615658</v>
       </c>
       <c r="D68" s="1">
         <f t="shared" si="1"/>
@@ -4531,11 +4533,11 @@
       </c>
       <c r="B69" s="1">
         <f t="shared" si="3"/>
-        <v>658924.73681203474</v>
+        <v>585642.50927413756</v>
       </c>
       <c r="C69" s="1">
         <f t="shared" si="0"/>
-        <v>19767.742104361041</v>
+        <v>17569.275278224126</v>
       </c>
       <c r="D69" s="1">
         <f t="shared" si="1"/>
@@ -4549,11 +4551,11 @@
       </c>
       <c r="B70" s="1">
         <f t="shared" si="3"/>
-        <v>653692.4789163958</v>
+        <v>578211.7845523617</v>
       </c>
       <c r="C70" s="1">
         <f t="shared" si="0"/>
-        <v>19610.774367491875</v>
+        <v>17346.353536570852</v>
       </c>
       <c r="D70" s="1">
         <f t="shared" si="1"/>
@@ -4567,11 +4569,11 @@
       </c>
       <c r="B71" s="1">
         <f t="shared" si="3"/>
-        <v>648303.25328388764</v>
+        <v>570558.13808893249</v>
       </c>
       <c r="C71" s="1">
         <f t="shared" si="0"/>
-        <v>19449.09759851663</v>
+        <v>17116.744142667972</v>
       </c>
       <c r="D71" s="1">
         <f t="shared" si="1"/>
@@ -4585,11 +4587,11 @@
       </c>
       <c r="B72" s="1">
         <f t="shared" si="3"/>
-        <v>642752.35088240425</v>
+        <v>562674.88223160047</v>
       </c>
       <c r="C72" s="1">
         <f t="shared" si="0"/>
-        <v>19282.570526472125</v>
+        <v>16880.246466948014</v>
       </c>
       <c r="D72" s="1">
         <f t="shared" si="1"/>
@@ -4603,11 +4605,11 @@
       </c>
       <c r="B73" s="1">
         <f t="shared" si="3"/>
-        <v>637034.92140887643</v>
+        <v>554555.12869854853</v>
       </c>
       <c r="C73" s="1">
         <f t="shared" si="0"/>
-        <v>19111.04764226629</v>
+        <v>16636.653860956456</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" si="1"/>
@@ -4621,11 +4623,11 @@
       </c>
       <c r="B74" s="1">
         <f t="shared" si="3"/>
-        <v>631145.96905114269</v>
+        <v>546191.78255950497</v>
       </c>
       <c r="C74" s="1">
         <f t="shared" si="0"/>
-        <v>18934.37907153428</v>
+        <v>16385.753476785147</v>
       </c>
       <c r="D74" s="1">
         <f t="shared" si="1"/>
@@ -4639,11 +4641,11 @@
       </c>
       <c r="B75" s="1">
         <f t="shared" si="3"/>
-        <v>625080.34812267695</v>
+        <v>537577.53603629011</v>
       </c>
       <c r="C75" s="1">
         <f t="shared" si="0"/>
-        <v>18752.410443680306</v>
+        <v>16127.326081088702</v>
       </c>
       <c r="D75" s="1">
         <f t="shared" si="1"/>
@@ -4657,11 +4659,11 @@
       </c>
       <c r="B76" s="1">
         <f t="shared" si="3"/>
-        <v>618832.75856635731</v>
+        <v>528704.86211737886</v>
       </c>
       <c r="C76" s="1">
         <f t="shared" si="0"/>
-        <v>18564.982756990717</v>
+        <v>15861.145863521366</v>
       </c>
       <c r="D76" s="1">
         <f t="shared" si="1"/>
@@ -4675,14 +4677,14 @@
       </c>
       <c r="B77" s="1">
         <f t="shared" si="3"/>
-        <v>612397.74132334802</v>
+        <v>519566.00798090023</v>
       </c>
       <c r="C77" s="1">
         <f t="shared" ref="C77:C88" si="4">B77*$B$7</f>
-        <v>18371.93223970044</v>
+        <v>15586.980239427006</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" ref="D77:D88" si="5">IF(A77&lt;=$B$4,$B$8,-$B$9)</f>
+        <f t="shared" si="1"/>
         <v>-25000</v>
       </c>
     </row>
@@ -4693,14 +4695,14 @@
       </c>
       <c r="B78" s="1">
         <f t="shared" si="3"/>
-        <v>605769.67356304848</v>
+        <v>510152.98822032718</v>
       </c>
       <c r="C78" s="1">
         <f t="shared" si="4"/>
-        <v>18173.090206891455</v>
+        <v>15304.589646609815</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D78:D88" si="5">IF(A78&lt;$B$4,$B$8,-$B$9)</f>
         <v>-25000</v>
       </c>
     </row>
@@ -4711,11 +4713,11 @@
       </c>
       <c r="B79" s="1">
         <f t="shared" si="3"/>
-        <v>598942.76376993989</v>
+        <v>500457.57786693703</v>
       </c>
       <c r="C79" s="1">
         <f t="shared" si="4"/>
-        <v>17968.282913098195</v>
+        <v>15013.727336008111</v>
       </c>
       <c r="D79" s="1">
         <f t="shared" si="5"/>
@@ -4729,11 +4731,11 @@
       </c>
       <c r="B80" s="1">
         <f t="shared" ref="B80:B88" si="7">B79+C79+D79</f>
-        <v>591911.04668303812</v>
+        <v>490471.30520294514</v>
       </c>
       <c r="C80" s="1">
         <f t="shared" si="4"/>
-        <v>17757.331400491144</v>
+        <v>14714.139156088353</v>
       </c>
       <c r="D80" s="1">
         <f t="shared" si="5"/>
@@ -4747,11 +4749,11 @@
       </c>
       <c r="B81" s="1">
         <f t="shared" si="7"/>
-        <v>584668.3780835293</v>
+        <v>480185.44435903348</v>
       </c>
       <c r="C81" s="1">
         <f t="shared" si="4"/>
-        <v>17540.051342505878</v>
+        <v>14405.563330771003</v>
       </c>
       <c r="D81" s="1">
         <f t="shared" si="5"/>
@@ -4765,11 +4767,11 @@
       </c>
       <c r="B82" s="1">
         <f t="shared" si="7"/>
-        <v>577208.42942603515</v>
+        <v>469591.00768980448</v>
       </c>
       <c r="C82" s="1">
         <f t="shared" si="4"/>
-        <v>17316.252882781053</v>
+        <v>14087.730230694135</v>
       </c>
       <c r="D82" s="1">
         <f t="shared" si="5"/>
@@ -4783,11 +4785,11 @@
       </c>
       <c r="B83" s="1">
         <f t="shared" si="7"/>
-        <v>569524.68230881623</v>
+        <v>458678.73792049859</v>
       </c>
       <c r="C83" s="1">
         <f t="shared" si="4"/>
-        <v>17085.740469264485</v>
+        <v>13760.362137614957</v>
       </c>
       <c r="D83" s="1">
         <f t="shared" si="5"/>
@@ -4801,11 +4803,11 @@
       </c>
       <c r="B84" s="1">
         <f t="shared" si="7"/>
-        <v>561610.42277808068</v>
+        <v>447439.10005811357</v>
       </c>
       <c r="C84" s="1">
         <f t="shared" si="4"/>
-        <v>16848.312683342421</v>
+        <v>13423.173001743407</v>
       </c>
       <c r="D84" s="1">
         <f t="shared" si="5"/>
@@ -4819,11 +4821,11 @@
       </c>
       <c r="B85" s="1">
         <f t="shared" si="7"/>
-        <v>553458.73546142306</v>
+        <v>435862.27305985696</v>
       </c>
       <c r="C85" s="1">
         <f t="shared" si="4"/>
-        <v>16603.762063842692</v>
+        <v>13075.868191795709</v>
       </c>
       <c r="D85" s="1">
         <f t="shared" si="5"/>
@@ -4837,11 +4839,11 @@
       </c>
       <c r="B86" s="1">
         <f t="shared" si="7"/>
-        <v>545062.49752526579</v>
+        <v>423938.14125165268</v>
       </c>
       <c r="C86" s="1">
         <f t="shared" si="4"/>
-        <v>16351.874925757973</v>
+        <v>12718.144237549579</v>
       </c>
       <c r="D86" s="1">
         <f t="shared" si="5"/>
@@ -4855,11 +4857,11 @@
       </c>
       <c r="B87" s="1">
         <f t="shared" si="7"/>
-        <v>536414.37245102378</v>
+        <v>411656.28548920224</v>
       </c>
       <c r="C87" s="1">
         <f t="shared" si="4"/>
-        <v>16092.431173530713</v>
+        <v>12349.688564676067</v>
       </c>
       <c r="D87" s="1">
         <f t="shared" si="5"/>
@@ -4873,11 +4875,11 @@
       </c>
       <c r="B88" s="1">
         <f t="shared" si="7"/>
-        <v>527506.80362455454</v>
+        <v>399005.97405387834</v>
       </c>
       <c r="C88" s="1">
         <f t="shared" si="4"/>
-        <v>15825.204108736636</v>
+        <v>11970.17922161635</v>
       </c>
       <c r="D88" s="1">
         <f t="shared" si="5"/>

</xml_diff>